<commit_message>
Atualização e inclusão de projetos
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3101239b6ba711c6/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{C5557F48-1AD3-4C29-BA07-55769A052356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C450C83-F4F9-48D1-BECC-D4FB9DDD5B86}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="8_{C5557F48-1AD3-4C29-BA07-55769A052356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1582872F-6E9C-47AD-9D8C-BC13F9219447}"/>
   <bookViews>
-    <workbookView xWindow="23010" yWindow="0" windowWidth="28590" windowHeight="21000" xr2:uid="{94DCEDE3-CC34-4AC9-BA0F-B867C8321C4B}"/>
+    <workbookView xWindow="19620" yWindow="1170" windowWidth="22935" windowHeight="16305" xr2:uid="{94DCEDE3-CC34-4AC9-BA0F-B867C8321C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="36">
   <si>
     <t>Flexor</t>
   </si>
@@ -82,6 +82,57 @@
   </si>
   <si>
     <t>Agarrar Esfera</t>
+  </si>
+  <si>
+    <t>RESULTADOS</t>
+  </si>
+  <si>
+    <t>Acertos</t>
+  </si>
+  <si>
+    <t>Erros</t>
+  </si>
+  <si>
+    <t>Outros Movimentos Detectados</t>
+  </si>
+  <si>
+    <t>Incerteza</t>
+  </si>
+  <si>
+    <t>Flex (10),  Pinça (6),  Flex.MI (4), Ext.Pol (4), Flex.MA (2),  Flex.Pol (2),  Joinha (2)</t>
+  </si>
+  <si>
+    <t>Acurácia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>Flex(16), Flex.Pol(4), Ext.Pol(4), Joinha(4), Flex.MA(3), Flex.MI(1)</t>
+  </si>
+  <si>
+    <t>Flex.Pol(6), Flex.MA(4), Flex.MI(3), Joinha(1), Agarrar(1)</t>
+  </si>
+  <si>
+    <t>Flex(15), Joinha(9), Pinça(4), Flex.MI(2),  Flex.Pol(1)</t>
+  </si>
+  <si>
+    <t>Joinha(5), Flex.Pol(5), Pinça(5),  Pinça(5),  Ext(3), Flex.MI(2), Agarrar(2), Ext.Pol(1)</t>
+  </si>
+  <si>
+    <t>Flex(14), Flex.MA(4), Flex.Pol(2),  Agarrar(2), Pinça(2), Ext (1), Flex.MI(1)</t>
+  </si>
+  <si>
+    <t>Joinha(5),  Agarrar(4), Flex(4), Flex.MI(3), Flex.Pol(2),  Pinça(1)</t>
+  </si>
+  <si>
+    <t>Joinha(6), Flex(1),  Ext(1), Flex.Pol(1), Ext.Pol(1), Pinça(1)</t>
+  </si>
+  <si>
+    <t>Ext.Pol(3), Agarrar(2), Flex.MI(2), Joinha(2), Flex.MA(1), Flex(1)</t>
+  </si>
+  <si>
+    <t>RESULTADOS (%)</t>
   </si>
 </sst>
 </file>
@@ -105,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +199,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -229,11 +292,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,6 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,8 +356,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0C2E0E-3D30-4240-8D1E-9E945E585204}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31:H39"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,39 +715,63 @@
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="23.42578125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="72.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="F2" s="11" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="F2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
+      <c r="K2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -657,8 +796,20 @@
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2">
+        <v>73</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="28"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="26"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -683,8 +834,22 @@
       <c r="I4" s="2">
         <v>42.71</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>21</v>
+      </c>
+      <c r="M4" s="23">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="27"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -703,14 +868,28 @@
       <c r="G5">
         <v>844.93</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>3300</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>132.16</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="23">
+        <v>6</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="26"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -735,8 +914,22 @@
       <c r="I6" s="2">
         <v>138.61000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="23">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="27"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -761,8 +954,22 @@
       <c r="I7" s="2">
         <v>128.13</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+      <c r="M7" s="23">
+        <v>8</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="16"/>
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -787,8 +994,22 @@
       <c r="I8" s="2">
         <v>126.52</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8" s="23">
+        <v>8</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="27"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -813,8 +1034,22 @@
       <c r="I9" s="2">
         <v>127.33</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="2">
+        <v>7</v>
+      </c>
+      <c r="M9" s="23">
+        <v>6</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="27"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -839,8 +1074,22 @@
       <c r="I10" s="2">
         <v>145.86000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="2">
+        <v>3</v>
+      </c>
+      <c r="M10" s="23">
+        <v>11</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="16"/>
+      <c r="P10" s="27"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -865,8 +1114,22 @@
       <c r="I11" s="2">
         <v>128.94</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="2">
+        <v>7</v>
+      </c>
+      <c r="M11" s="23">
+        <v>13</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="27"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -891,31 +1154,52 @@
       <c r="I12" s="2">
         <v>125.71</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="23">
+        <v>11</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="27"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="2">
         <v>342.75</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="2">
         <v>813.11</v>
       </c>
       <c r="I13" s="2">
         <v>130.55000000000001</v>
       </c>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="K14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -928,14 +1212,27 @@
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="K15" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="29"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -960,8 +1257,21 @@
       <c r="I16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="20">
+        <v>1</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="28">
+        <v>0</v>
+      </c>
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -986,8 +1296,21 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="22">
+        <v>0.4118</v>
+      </c>
+      <c r="M17" s="24">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="N17" s="22">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1012,8 +1335,21 @@
       <c r="I18" s="2">
         <v>5.64</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="20">
+        <v>0</v>
+      </c>
+      <c r="M18" s="24">
+        <v>0.16220000000000001</v>
+      </c>
+      <c r="N18" s="22">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="O18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1038,8 +1374,21 @@
       <c r="I19" s="2">
         <v>12.89</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="22">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="M19" s="24">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="N19" s="22">
+        <v>0.37930000000000003</v>
+      </c>
+      <c r="O19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1064,8 +1413,21 @@
       <c r="I20" s="2">
         <v>5.64</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0.1154</v>
+      </c>
+      <c r="M20" s="24">
+        <v>0.30769999999999997</v>
+      </c>
+      <c r="N20" s="22">
+        <v>0.57689999999999997</v>
+      </c>
+      <c r="O20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1090,8 +1452,21 @@
       <c r="I21" s="2">
         <v>5.64</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="22">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="M21" s="24">
+        <v>0.1905</v>
+      </c>
+      <c r="N21" s="22">
+        <v>0.76190000000000002</v>
+      </c>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1116,8 +1491,21 @@
       <c r="I22" s="2">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="22">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="M22" s="24">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="N22" s="22">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="O22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1142,8 +1530,21 @@
       <c r="I23" s="2">
         <v>12.09</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" s="22">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="M23" s="24">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="N23" s="22">
+        <v>0.57569999999999999</v>
+      </c>
+      <c r="O23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1168,8 +1569,21 @@
       <c r="I24" s="2">
         <v>12.89</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="22">
+        <v>0.2258</v>
+      </c>
+      <c r="M24" s="24">
+        <v>0.4194</v>
+      </c>
+      <c r="N24" s="22">
+        <v>0.3548</v>
+      </c>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1182,14 +1596,27 @@
       <c r="I25" s="2">
         <v>8.86</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="K25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" s="22">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="M25" s="24">
+        <v>0.26190000000000002</v>
+      </c>
+      <c r="N25" s="22">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
       <c r="F26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1630,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1230,14 +1657,14 @@
       <c r="D28" s="2">
         <v>27.4</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -1263,7 +1690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -1288,9 +1715,8 @@
       <c r="I30" s="2">
         <v>361.03</v>
       </c>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1742,7 @@
         <v>456.92</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1335,7 +1761,7 @@
       <c r="G32" s="2">
         <v>1418.71</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="5">
         <v>3300</v>
       </c>
       <c r="I32" s="2">
@@ -1489,7 +1915,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K14:N14"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A2:D2"/>
@@ -1497,7 +1926,6 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F28:I28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>